<commit_message>
refactor: create core Dataset object; major breaking changes everywhere
</commit_message>
<xml_diff>
--- a/tests/cli/merge/small_expected_results.xlsx
+++ b/tests/cli/merge/small_expected_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alee7/ucsf/git/macpie/tests/cli/merge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83680132-213A-9344-B09F-D0015E83BE7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C36A689-BB1E-9447-9893-4BBC019E3173}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16540" yWindow="5180" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MERGED_RESULTS" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,14 @@
     <sheet name="_sheets" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MERGED_RESULTS!$B$2:$X$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MERGED_RESULTS!$B$2:$S$27</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="78">
   <si>
     <t>small</t>
   </si>
@@ -50,15 +50,6 @@
     <t>InstrID</t>
   </si>
   <si>
-    <t>link_date</t>
-  </si>
-  <si>
-    <t>link_id</t>
-  </si>
-  <si>
-    <t>DCStatus</t>
-  </si>
-  <si>
     <t>Col1</t>
   </si>
   <si>
@@ -66,12 +57,6 @@
   </si>
   <si>
     <t>Col3</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>Unknown</t>
   </si>
   <si>
     <t>sheetname</t>
@@ -671,15 +656,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -688,30 +686,25 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
       <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="5"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="5"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -734,58 +727,43 @@
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="Q2" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="T2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -798,26 +776,17 @@
       <c r="D3">
         <v>178771</v>
       </c>
-      <c r="E3" s="2">
-        <v>36452</v>
+      <c r="E3">
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>178771</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -830,68 +799,53 @@
       <c r="D4">
         <v>877207</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>212592</v>
+      </c>
+      <c r="I4" s="2">
         <v>35912</v>
       </c>
-      <c r="F4">
-        <v>877207</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
       <c r="J4">
-        <v>1</v>
+        <v>500861</v>
       </c>
       <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
         <v>212592</v>
       </c>
-      <c r="L4" s="2">
+      <c r="O4" s="2">
         <v>35912</v>
       </c>
-      <c r="M4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4">
-        <v>500861</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
       <c r="P4">
-        <v>1</v>
+        <v>603240</v>
       </c>
       <c r="Q4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R4">
-        <v>212592</v>
-      </c>
-      <c r="S4" s="2">
-        <v>35912</v>
-      </c>
-      <c r="T4" t="s">
-        <v>13</v>
-      </c>
-      <c r="U4">
-        <v>603240</v>
-      </c>
-      <c r="V4">
-        <v>1</v>
-      </c>
-      <c r="W4">
-        <v>1</v>
-      </c>
-      <c r="X4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -904,68 +858,53 @@
       <c r="D5">
         <v>925508</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>225430</v>
+      </c>
+      <c r="I5" s="2">
         <v>35547</v>
       </c>
-      <c r="F5">
-        <v>925508</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
       <c r="J5">
-        <v>1</v>
+        <v>888874</v>
       </c>
       <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
         <v>225430</v>
       </c>
-      <c r="L5" s="2">
+      <c r="O5" s="2">
         <v>35547</v>
       </c>
-      <c r="M5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5">
-        <v>888874</v>
-      </c>
-      <c r="O5">
-        <v>2</v>
-      </c>
       <c r="P5">
-        <v>0</v>
+        <v>341269</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R5">
-        <v>225430</v>
-      </c>
-      <c r="S5" s="2">
-        <v>35547</v>
-      </c>
-      <c r="T5" t="s">
-        <v>13</v>
-      </c>
-      <c r="U5">
-        <v>341269</v>
-      </c>
-      <c r="V5">
-        <v>2</v>
-      </c>
-      <c r="W5">
         <v>-6</v>
       </c>
-      <c r="X5">
+      <c r="S5">
         <v>-6</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -978,26 +917,17 @@
       <c r="D6">
         <v>499743</v>
       </c>
-      <c r="E6" s="2">
-        <v>35614</v>
+      <c r="E6">
+        <v>0.5</v>
       </c>
       <c r="F6">
-        <v>499743</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <v>0.5</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1010,26 +940,17 @@
       <c r="D7">
         <v>779189</v>
       </c>
-      <c r="E7" s="2">
-        <v>35900</v>
+      <c r="E7">
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>779189</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1042,26 +963,17 @@
       <c r="D8">
         <v>137398</v>
       </c>
-      <c r="E8" s="2">
-        <v>35679</v>
+      <c r="E8">
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>137398</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1074,26 +986,17 @@
       <c r="D9">
         <v>515744</v>
       </c>
-      <c r="E9" s="2">
-        <v>35666</v>
+      <c r="E9">
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>515744</v>
-      </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
         <v>-9</v>
       </c>
-      <c r="J9">
+      <c r="G9">
         <v>-9</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1106,26 +1009,17 @@
       <c r="D10">
         <v>187481</v>
       </c>
-      <c r="E10" s="2">
-        <v>39230</v>
+      <c r="E10">
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>187481</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="G10">
         <v>0</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1138,26 +1032,17 @@
       <c r="D11">
         <v>250964</v>
       </c>
-      <c r="E11" s="2">
-        <v>35593</v>
+      <c r="E11">
+        <v>0.5</v>
       </c>
       <c r="F11">
-        <v>250964</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="G11">
         <v>0.5</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1170,26 +1055,17 @@
       <c r="D12">
         <v>185271</v>
       </c>
-      <c r="E12" s="2">
-        <v>35982</v>
+      <c r="E12">
+        <v>0.5</v>
       </c>
       <c r="F12">
-        <v>185271</v>
-      </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12">
         <v>0.5</v>
       </c>
-      <c r="I12">
+      <c r="G12">
         <v>0.5</v>
       </c>
-      <c r="J12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1202,26 +1078,17 @@
       <c r="D13">
         <v>785354</v>
       </c>
-      <c r="E13" s="2">
-        <v>35617</v>
+      <c r="E13">
+        <v>0.5</v>
       </c>
       <c r="F13">
-        <v>785354</v>
-      </c>
-      <c r="G13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13">
-        <v>0.5</v>
-      </c>
-      <c r="I13">
         <v>0</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1234,47 +1101,35 @@
       <c r="D14">
         <v>104467</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14">
+        <v>0.5</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0.5</v>
+      </c>
+      <c r="H14">
+        <v>525567</v>
+      </c>
+      <c r="I14" s="2">
         <v>36410</v>
       </c>
-      <c r="F14">
-        <v>104467</v>
-      </c>
-      <c r="G14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14">
-        <v>0.5</v>
-      </c>
-      <c r="I14">
+      <c r="J14">
+        <v>671290</v>
+      </c>
+      <c r="K14">
         <v>0</v>
       </c>
-      <c r="J14">
-        <v>0.5</v>
-      </c>
-      <c r="K14">
-        <v>525567</v>
-      </c>
-      <c r="L14" s="2">
-        <v>36410</v>
-      </c>
-      <c r="M14" t="s">
-        <v>13</v>
-      </c>
-      <c r="N14">
-        <v>671290</v>
-      </c>
-      <c r="O14">
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
         <v>0</v>
       </c>
-      <c r="P14">
-        <v>1</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1287,26 +1142,17 @@
       <c r="D15">
         <v>819165</v>
       </c>
-      <c r="E15" s="2">
-        <v>35708</v>
+      <c r="E15">
+        <v>2</v>
       </c>
       <c r="F15">
-        <v>819165</v>
-      </c>
-      <c r="G15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="J15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1319,26 +1165,17 @@
       <c r="D16">
         <v>617550</v>
       </c>
-      <c r="E16" s="2">
-        <v>36069</v>
+      <c r="E16">
+        <v>1</v>
       </c>
       <c r="F16">
-        <v>617550</v>
-      </c>
-      <c r="G16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1351,68 +1188,53 @@
       <c r="D17">
         <v>488606</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0.5</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>584891</v>
+      </c>
+      <c r="I17" s="2">
         <v>37230</v>
       </c>
-      <c r="F17">
-        <v>488606</v>
-      </c>
-      <c r="G17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>0.5</v>
-      </c>
       <c r="J17">
-        <v>1</v>
+        <v>190736</v>
       </c>
       <c r="K17">
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <v>3</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
         <v>584891</v>
       </c>
-      <c r="L17" s="2">
+      <c r="O17" s="2">
         <v>37230</v>
       </c>
-      <c r="M17" t="s">
-        <v>13</v>
-      </c>
-      <c r="N17">
-        <v>190736</v>
-      </c>
-      <c r="O17">
-        <v>3</v>
-      </c>
       <c r="P17">
-        <v>3</v>
+        <v>994547</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R17">
-        <v>584891</v>
-      </c>
-      <c r="S17" s="2">
-        <v>37230</v>
-      </c>
-      <c r="T17" t="s">
-        <v>13</v>
-      </c>
-      <c r="U17">
-        <v>994547</v>
-      </c>
-      <c r="V17">
-        <v>2</v>
-      </c>
-      <c r="W17">
         <v>-6</v>
       </c>
-      <c r="X17">
+      <c r="S17">
         <v>-6</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1425,41 +1247,26 @@
       <c r="D18">
         <v>613114</v>
       </c>
-      <c r="E18" s="2">
+      <c r="H18">
+        <v>645686</v>
+      </c>
+      <c r="I18" s="2">
         <v>37435</v>
       </c>
-      <c r="F18">
-        <v>613114</v>
-      </c>
-      <c r="G18" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18">
+      <c r="J18">
+        <v>877446</v>
+      </c>
+      <c r="N18">
         <v>645686</v>
       </c>
-      <c r="L18" s="2">
+      <c r="O18" s="2">
         <v>37435</v>
       </c>
-      <c r="M18" t="s">
-        <v>14</v>
-      </c>
-      <c r="N18">
-        <v>877446</v>
-      </c>
-      <c r="R18">
-        <v>645686</v>
-      </c>
-      <c r="S18" s="2">
-        <v>37435</v>
-      </c>
-      <c r="T18" t="s">
-        <v>14</v>
-      </c>
-      <c r="U18">
+      <c r="P18">
         <v>768903</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1472,26 +1279,17 @@
       <c r="D19">
         <v>207261</v>
       </c>
-      <c r="E19" s="2">
-        <v>35680</v>
+      <c r="E19">
+        <v>2</v>
       </c>
       <c r="F19">
-        <v>207261</v>
-      </c>
-      <c r="G19" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19">
-        <v>2</v>
-      </c>
-      <c r="I19">
-        <v>2</v>
-      </c>
-      <c r="J19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1504,26 +1302,17 @@
       <c r="D20">
         <v>715059</v>
       </c>
-      <c r="E20" s="2">
-        <v>35837</v>
+      <c r="E20">
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>715059</v>
-      </c>
-      <c r="G20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
         <v>-9</v>
       </c>
-      <c r="J20">
+      <c r="G20">
         <v>-9</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1536,26 +1325,17 @@
       <c r="D21">
         <v>534853</v>
       </c>
-      <c r="E21" s="2">
-        <v>35431</v>
+      <c r="E21">
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>534853</v>
-      </c>
-      <c r="G21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <v>2</v>
-      </c>
-      <c r="J21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1568,26 +1348,17 @@
       <c r="D22">
         <v>497023</v>
       </c>
-      <c r="E22" s="2">
-        <v>35990</v>
+      <c r="E22">
+        <v>2</v>
       </c>
       <c r="F22">
-        <v>497023</v>
-      </c>
-      <c r="G22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22">
-        <v>2</v>
-      </c>
-      <c r="I22">
-        <v>2</v>
-      </c>
-      <c r="J22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1600,26 +1371,17 @@
       <c r="D23">
         <v>744447</v>
       </c>
-      <c r="E23" s="2">
-        <v>35607</v>
+      <c r="E23">
+        <v>0.5</v>
       </c>
       <c r="F23">
-        <v>744447</v>
-      </c>
-      <c r="G23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="G23">
         <v>0.5</v>
       </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1632,68 +1394,53 @@
       <c r="D24">
         <v>523686</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>899113</v>
+      </c>
+      <c r="I24" s="2">
         <v>35950</v>
       </c>
-      <c r="F24">
-        <v>523686</v>
-      </c>
-      <c r="G24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24">
-        <v>2</v>
-      </c>
-      <c r="I24">
-        <v>2</v>
-      </c>
       <c r="J24">
-        <v>2</v>
+        <v>448547</v>
       </c>
       <c r="K24">
+        <v>3</v>
+      </c>
+      <c r="L24">
+        <v>3</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
         <v>899113</v>
       </c>
-      <c r="L24" s="2">
+      <c r="O24" s="2">
         <v>35950</v>
       </c>
-      <c r="M24" t="s">
-        <v>13</v>
-      </c>
-      <c r="N24">
-        <v>448547</v>
-      </c>
-      <c r="O24">
-        <v>3</v>
-      </c>
       <c r="P24">
-        <v>3</v>
+        <v>671293</v>
       </c>
       <c r="Q24">
         <v>1</v>
       </c>
       <c r="R24">
-        <v>899113</v>
-      </c>
-      <c r="S24" s="2">
-        <v>35950</v>
-      </c>
-      <c r="T24" t="s">
-        <v>13</v>
-      </c>
-      <c r="U24">
-        <v>671293</v>
-      </c>
-      <c r="V24">
-        <v>1</v>
-      </c>
-      <c r="W24">
-        <v>2</v>
-      </c>
-      <c r="X24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="S24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1706,68 +1453,53 @@
       <c r="D25">
         <v>792204</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <v>922196</v>
+      </c>
+      <c r="I25" s="2">
         <v>36020</v>
       </c>
-      <c r="F25">
-        <v>792204</v>
-      </c>
-      <c r="G25" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25">
-        <v>2</v>
-      </c>
-      <c r="I25">
-        <v>2</v>
-      </c>
       <c r="J25">
+        <v>383441</v>
+      </c>
+      <c r="K25">
         <v>3</v>
       </c>
-      <c r="K25">
+      <c r="L25">
+        <v>3</v>
+      </c>
+      <c r="M25">
+        <v>3</v>
+      </c>
+      <c r="N25">
         <v>922196</v>
       </c>
-      <c r="L25" s="2">
+      <c r="O25" s="2">
         <v>36020</v>
       </c>
-      <c r="M25" t="s">
-        <v>13</v>
-      </c>
-      <c r="N25">
-        <v>383441</v>
-      </c>
-      <c r="O25">
-        <v>3</v>
-      </c>
       <c r="P25">
-        <v>3</v>
+        <v>363835</v>
       </c>
       <c r="Q25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R25">
-        <v>922196</v>
-      </c>
-      <c r="S25" s="2">
-        <v>36020</v>
-      </c>
-      <c r="T25" t="s">
-        <v>13</v>
-      </c>
-      <c r="U25">
-        <v>363835</v>
-      </c>
-      <c r="V25">
-        <v>2</v>
-      </c>
-      <c r="W25">
         <v>-6</v>
       </c>
-      <c r="X25">
+      <c r="S25">
         <v>-6</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1780,52 +1512,40 @@
       <c r="D26">
         <v>198487</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>936316</v>
+      </c>
+      <c r="O26" s="2">
         <v>37918</v>
       </c>
-      <c r="F26">
-        <v>198487</v>
-      </c>
-      <c r="G26" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-      <c r="J26">
-        <v>1</v>
+      <c r="P26">
+        <v>443633</v>
+      </c>
+      <c r="Q26">
+        <v>2</v>
       </c>
       <c r="R26">
-        <v>936316</v>
-      </c>
-      <c r="S26" s="2">
-        <v>37918</v>
-      </c>
-      <c r="T26" t="s">
-        <v>13</v>
-      </c>
-      <c r="U26">
-        <v>443633</v>
-      </c>
-      <c r="V26">
-        <v>2</v>
-      </c>
-      <c r="W26">
         <v>-6</v>
       </c>
-      <c r="X26">
+      <c r="S26">
         <v>-6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:X27" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B2:S27" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="3">
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="K1:Q1"/>
-    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:S1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1848,82 +1568,82 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1947,121 +1667,121 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
-        <v>47</v>
-      </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2083,42 +1803,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2146,162 +1866,162 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" t="s">
         <v>72</v>
       </c>
-      <c r="E3" t="s">
+      <c r="J3" t="s">
         <v>73</v>
-      </c>
-      <c r="F3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3" t="s">
-        <v>77</v>
-      </c>
-      <c r="J3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" t="s">
         <v>73</v>
       </c>
-      <c r="F4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>75</v>
-      </c>
-      <c r="H4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I4" t="s">
-        <v>78</v>
-      </c>
-      <c r="J4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>